<commit_message>
quality of life improvements
</commit_message>
<xml_diff>
--- a/benchmarks-lrp.xlsx
+++ b/benchmarks-lrp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Academia\Research\dev\LRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CED6F5-D90B-4BD5-90D9-4865AED27A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EDB594-99DF-41AD-AC09-8CA637D0E8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="2" r:id="rId1"/>
@@ -246,13 +246,7 @@
     <t>            μ̲   =   0.1                     ,</t>
   </si>
   <si>
-    <t>            C̲   =   4                       ,</t>
-  </si>
-  <si>
     <t>            μ̅   =   0.4                     ,</t>
-  </si>
-  <si>
-    <t>            C̅   =   60                      ,</t>
   </si>
   <si>
     <t>            ρ   =   0.1</t>
@@ -375,6 +369,12 @@
   </si>
   <si>
     <t>16.0 GB</t>
+  </si>
+  <si>
+    <t>            c̲   =   4                       ,</t>
+  </si>
+  <si>
+    <t>            c̅   =   60                      ,</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5551421D-4FE7-47B7-A546-15E7A05240A9}">
   <dimension ref="A1:V287"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1186,7 +1186,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
@@ -1199,7 +1199,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
@@ -1230,7 +1230,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1284,7 +1284,7 @@
         <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="19" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B19" s="19"/>
       <c r="K19" s="1"/>
@@ -1333,14 +1333,14 @@
     </row>
     <row r="21" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1349,14 +1349,14 @@
     </row>
     <row r="22" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1364,14 +1364,14 @@
     </row>
     <row r="23" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1384,14 +1384,14 @@
     </row>
     <row r="24" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1407,7 +1407,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1741,7 +1741,7 @@
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -1918,7 +1918,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="50" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="51" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="52" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2032,7 +2032,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2049,7 +2049,7 @@
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -2069,7 +2069,7 @@
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -2084,7 +2084,7 @@
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -2092,14 +2092,14 @@
     </row>
     <row r="58" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="22" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -2107,14 +2107,14 @@
     </row>
     <row r="59" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -2122,14 +2122,14 @@
     </row>
     <row r="60" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="22" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -2137,14 +2137,14 @@
     </row>
     <row r="61" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -2159,7 +2159,7 @@
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -2174,35 +2174,35 @@
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -2210,14 +2210,14 @@
     </row>
     <row r="66" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -2853,7 +2853,7 @@
       <c r="K1" s="37"/>
       <c r="L1" s="38"/>
       <c r="N1" s="36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O1" s="37"/>
       <c r="P1" s="37"/>
@@ -3828,7 +3828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348A00D3-4455-4871-A842-3FB0F610BDD7}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -3857,10 +3857,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" s="48" t="s">
         <v>1</v>
@@ -3868,7 +3868,7 @@
       <c r="E2" s="46"/>
       <c r="F2" s="47"/>
       <c r="G2" s="49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.45">

</xml_diff>